<commit_message>
1. Finer tuning/modifications on Mode 4 - seeks for broader spaces by default when goal is not visible 2. Modified algorithm for goal selection - more chance for the goal to be reachable 3. Now program automatically collects data and concatenates with already existing data
</commit_message>
<xml_diff>
--- a/mazeLib/maze2.xlsx
+++ b/mazeLib/maze2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chansol-RIT\Documents\MATLAB\RNN_Classifier\mazeLib\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7935"/>
   </bookViews>
@@ -16,8 +21,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,8 +30,14 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -42,12 +53,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -162,20 +167,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,9 +225,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,9 +259,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,9 +294,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="CY60" sqref="CY60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BV49" sqref="BV49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6447,8 +6461,8 @@
       <c r="CB20" s="5">
         <v>0</v>
       </c>
-      <c r="CC20" s="2">
-        <v>107</v>
+      <c r="CC20" s="5">
+        <v>0</v>
       </c>
       <c r="CD20" s="5">
         <v>0</v>
@@ -7021,8 +7035,8 @@
       <c r="BR22" s="5">
         <v>0</v>
       </c>
-      <c r="BS22" s="5">
-        <v>0</v>
+      <c r="BS22" s="2">
+        <v>109</v>
       </c>
       <c r="BT22" s="5">
         <v>0</v>
@@ -7643,8 +7657,8 @@
       <c r="BX24" s="5">
         <v>0</v>
       </c>
-      <c r="BY24" s="5">
-        <v>0</v>
+      <c r="BY24" s="2">
+        <v>108</v>
       </c>
       <c r="BZ24" s="5">
         <v>0</v>
@@ -8151,8 +8165,8 @@
       <c r="AR26" s="5">
         <v>0</v>
       </c>
-      <c r="AS26" s="16">
-        <v>208</v>
+      <c r="AS26" s="5">
+        <v>0</v>
       </c>
       <c r="AT26" s="5">
         <v>0</v>
@@ -9957,8 +9971,8 @@
       <c r="AP32" s="5">
         <v>0</v>
       </c>
-      <c r="AQ32" s="5">
-        <v>0</v>
+      <c r="AQ32" s="16">
+        <v>208</v>
       </c>
       <c r="AR32" s="5">
         <v>0</v>
@@ -10609,8 +10623,8 @@
       <c r="BF34" s="5">
         <v>0</v>
       </c>
-      <c r="BG34" s="2">
-        <v>109</v>
+      <c r="BG34" s="5">
+        <v>0</v>
       </c>
       <c r="BH34" s="5">
         <v>0</v>
@@ -12143,8 +12157,8 @@
       <c r="BN39" s="5">
         <v>0</v>
       </c>
-      <c r="BO39" s="2">
-        <v>108</v>
+      <c r="BO39" s="5">
+        <v>0</v>
       </c>
       <c r="BP39" s="5">
         <v>0</v>
@@ -13094,8 +13108,8 @@
       <c r="CC42" s="5">
         <v>0</v>
       </c>
-      <c r="CD42" s="5">
-        <v>0</v>
+      <c r="CD42" s="2">
+        <v>107</v>
       </c>
       <c r="CE42" s="5">
         <v>0</v>
@@ -15740,8 +15754,8 @@
       <c r="BE51" s="5">
         <v>0</v>
       </c>
-      <c r="BF51" s="17">
-        <v>205</v>
+      <c r="BF51" s="5">
+        <v>0</v>
       </c>
       <c r="BG51" s="5">
         <v>0</v>
@@ -17543,8 +17557,8 @@
       <c r="BB57" s="5">
         <v>0</v>
       </c>
-      <c r="BC57" s="5">
-        <v>0</v>
+      <c r="BC57" s="16">
+        <v>205</v>
       </c>
       <c r="BD57" s="5">
         <v>0</v>
@@ -20727,8 +20741,8 @@
       <c r="H68" s="5">
         <v>0</v>
       </c>
-      <c r="I68" s="5">
-        <v>0</v>
+      <c r="I68" s="2">
+        <v>115</v>
       </c>
       <c r="J68" s="5">
         <v>0</v>
@@ -22575,8 +22589,8 @@
       <c r="T74" s="5">
         <v>0</v>
       </c>
-      <c r="U74" s="2">
-        <v>115</v>
+      <c r="U74" s="5">
+        <v>0</v>
       </c>
       <c r="V74" s="5">
         <v>0</v>
@@ -22841,8 +22855,8 @@
       <c r="H75" s="5">
         <v>0</v>
       </c>
-      <c r="I75" s="5">
-        <v>0</v>
+      <c r="I75" s="2">
+        <v>116</v>
       </c>
       <c r="J75" s="5">
         <v>0</v>
@@ -24070,8 +24084,8 @@
       <c r="O79" s="5">
         <v>0</v>
       </c>
-      <c r="P79" s="2">
-        <v>116</v>
+      <c r="P79" s="5">
+        <v>0</v>
       </c>
       <c r="Q79" s="5">
         <v>0</v>
@@ -30670,31 +30684,35 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>